<commit_message>
added graphs in data
</commit_message>
<xml_diff>
--- a/task3/solution/Time.xlsx
+++ b/task3/solution/Time.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olegb\YandexDisk-berezin.op@phystech.edu\Учёба\CT\3_sem_22_23\task3\solution\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68EAC50C-FC2E-4E65-91E0-65A9DDEDD67D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8045AF92-80EF-4FF9-BC92-A66DAFF9D22D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,8 +16,21 @@
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Лист1!$K$20</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Лист1!$K$20</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">Лист1!$G$3:$H$3</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Лист1!$G$3:$I$3</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">Лист1!$G$3:$H$3</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">Лист1!$G$3:$I$3</definedName>
+    <definedName name="_xlchart.v1.12" hidden="1">Лист1!$I$3:$I$5</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">Лист1!$I$3:$I$6</definedName>
+    <definedName name="_xlchart.v1.14" hidden="1">Лист1!$K$20</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Лист1!$I$3:$I$5</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Лист1!$I$3:$I$6</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Лист1!$K$20</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">Лист1!$G$3:$H$3</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">Лист1!$G$3:$I$3</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">Лист1!$I$3:$I$5</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">Лист1!$I$3:$I$6</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">Лист1!$K$20</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="20">
   <si>
     <t>File size</t>
   </si>
@@ -162,60 +175,1710 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chartEx1.xml><?xml version="1.0" encoding="utf-8"?>
-<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
-  <cx:chartData>
-    <cx:data id="0">
-      <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.1</cx:f>
-      </cx:numDim>
-    </cx:data>
-  </cx:chartData>
-  <cx:chart>
-    <cx:title pos="t" align="ctr" overlay="0">
-      <cx:txPr>
-        <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>small file size</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
         <a:lstStyle/>
         <a:p>
-          <a:pPr algn="ctr" rtl="0">
-            <a:defRPr/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="ru-RU" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000">
+                <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
                   <a:lumOff val="35000"/>
-                </a:sysClr>
+                </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-            </a:rPr>
-            <a:t>Заголовок диаграммы</a:t>
-          </a:r>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
         </a:p>
-      </cx:txPr>
-    </cx:title>
-    <cx:plotArea>
-      <cx:plotAreaRegion>
-        <cx:series layoutId="clusteredColumn" uniqueId="{380DCE3C-C0E0-46FB-9022-4D90EF27F884}">
-          <cx:dataId val="0"/>
-          <cx:layoutPr>
-            <cx:binning intervalClosed="r"/>
-          </cx:layoutPr>
-        </cx:series>
-      </cx:plotAreaRegion>
-      <cx:axis id="0">
-        <cx:catScaling gapWidth="0"/>
-        <cx:tickLabels/>
-      </cx:axis>
-      <cx:axis id="1">
-        <cx:valScaling/>
-        <cx:majorGridlines/>
-        <cx:tickLabels/>
-      </cx:axis>
-    </cx:plotArea>
-  </cx:chart>
-</cx:chartSpace>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:view3D>
+      <c:rotX val="15"/>
+      <c:rotY val="20"/>
+      <c:depthPercent val="100"/>
+      <c:rAngAx val="1"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:backWall>
+    <c:plotArea>
+      <c:layout/>
+      <c:bar3DChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$K$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SMALL</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Лист1!$L$13:$N$13</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Shared Memory</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>msq</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>FIFO</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист1!$L$14:$N$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B5F1-4154-8CD9-EECC13D6CA12}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$K$15</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>MEDIUM</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Лист1!$L$13:$N$13</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Shared Memory</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>msq</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>FIFO</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист1!$L$15:$N$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-B5F1-4154-8CD9-EECC13D6CA12}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$K$16</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>BIG</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Лист1!$L$13:$N$13</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Shared Memory</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>msq</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>FIFO</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист1!$L$16:$N$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-B5F1-4154-8CD9-EECC13D6CA12}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:shape val="box"/>
+        <c:axId val="1568059152"/>
+        <c:axId val="1568059984"/>
+        <c:axId val="0"/>
+      </c:bar3DChart>
+      <c:catAx>
+        <c:axId val="1568059152"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1568059984"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1568059984"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>time</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="ru-RU"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1568059152"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ru-RU"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>medium</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> file size</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:view3D>
+      <c:rotX val="15"/>
+      <c:rotY val="20"/>
+      <c:depthPercent val="100"/>
+      <c:rAngAx val="1"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:backWall>
+    <c:plotArea>
+      <c:layout/>
+      <c:bar3DChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$K$19</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SMALL</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Лист1!$L$18:$N$18</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Shared Memory</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>msq</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>FIFO</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист1!$L$19:$N$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.09</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-FB92-496D-8903-122C25418F31}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$K$20</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>MEDIUM</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Лист1!$L$18:$N$18</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Shared Memory</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>msq</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>FIFO</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист1!$L$20:$N$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-FB92-496D-8903-122C25418F31}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$K$21</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>BIG</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Лист1!$L$18:$N$18</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Shared Memory</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>msq</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>FIFO</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист1!$L$21:$N$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-FB92-496D-8903-122C25418F31}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:shape val="box"/>
+        <c:axId val="1652269104"/>
+        <c:axId val="1652280336"/>
+        <c:axId val="0"/>
+      </c:bar3DChart>
+      <c:catAx>
+        <c:axId val="1652269104"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1652280336"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1652280336"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>time</a:t>
+                </a:r>
+                <a:endParaRPr lang="ru-RU"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="ru-RU"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1652269104"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ru-RU"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>big file size</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:view3D>
+      <c:rotX val="15"/>
+      <c:rotY val="20"/>
+      <c:depthPercent val="100"/>
+      <c:rAngAx val="1"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:backWall>
+    <c:plotArea>
+      <c:layout/>
+      <c:bar3DChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$K$35</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SMALL</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Лист1!$L$34:$N$34</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Shared Memory</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>msq</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>FIFO</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист1!$L$35:$N$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>8.3000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>108.56</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>97.22</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3A0A-4B0D-80B6-F67254E91D91}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$K$36</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>MEDIUM</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Лист1!$L$34:$N$34</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Shared Memory</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>msq</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>FIFO</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист1!$L$36:$N$36</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>2.0299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.66</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.4900000000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-3A0A-4B0D-80B6-F67254E91D91}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$K$37</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>BIG</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Лист1!$L$34:$N$34</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Shared Memory</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>msq</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>FIFO</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист1!$L$37:$N$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>2.65</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.14</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.86</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-3A0A-4B0D-80B6-F67254E91D91}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:shape val="box"/>
+        <c:axId val="1817959424"/>
+        <c:axId val="1817964000"/>
+        <c:axId val="0"/>
+      </c:bar3DChart>
+      <c:catAx>
+        <c:axId val="1817959424"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1817964000"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1817964000"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>time</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="ru-RU"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1817959424"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ru-RU"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
 </file>
 
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -258,8 +1921,88 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="366">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="286">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -270,7 +2013,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900"/>
+    <cs:defRPr sz="1000" kern="1200"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
@@ -282,7 +2025,19 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
@@ -293,30 +2048,7 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000"/>
+    <cs:defRPr sz="1000" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
@@ -324,11 +2056,11 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:dataLabel>
   <cs:dataLabelCallout>
     <cs:lnRef idx="0"/>
@@ -353,46 +2085,36 @@
         </a:solidFill>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900"/>
+    <cs:defRPr sz="900" kern="1200"/>
     <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
       <a:spAutoFit/>
     </cs:bodyPr>
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
+    <cs:fillRef idx="1"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
@@ -407,8 +2129,10 @@
     </cs:spPr>
   </cs:dataPointLine>
   <cs:dataPointMarker>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
@@ -416,12 +2140,9 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="lt1"/>
+          <a:schemeClr val="phClr"/>
         </a:solidFill>
       </a:ln>
     </cs:spPr>
@@ -431,13 +2152,13 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -456,38 +2177,41 @@
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900"/>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:dataTable>
   <cs:downBar>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -536,6 +2260,12 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
   </cs:floor>
   <cs:gridlineMajor>
     <cs:lnRef idx="0"/>
@@ -567,8 +2297,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -586,8 +2316,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -623,7 +2353,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:legend>
   <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
     <cs:lnRef idx="0"/>
@@ -651,18 +2381,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:seriesAxis>
   <cs:seriesLine>
     <cs:lnRef idx="0"/>
@@ -672,9 +2391,12 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat">
-        <a:solidFill>
-          <a:srgbClr val="D9D9D9"/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
@@ -690,7 +2412,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1400"/>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -706,7 +2428,7 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:prstDash val="sysDash"/>
+        <a:prstDash val="sysDot"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -720,30 +2442,225 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:trendlineLabel>
   <cs:upBar>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="286">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
@@ -753,7 +2670,307 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900"/>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
     <cs:lnRef idx="0"/>
@@ -762,6 +2979,506 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="286">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -770,80 +3487,110 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>198783</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>175591</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>6626</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>3313</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>159026</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>135835</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>311426</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>149086</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
-        <xdr:graphicFrame macro="">
-          <xdr:nvGraphicFramePr>
-            <xdr:cNvPr id="2" name="Диаграмма 1">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B33FBD22-A849-4D61-83BB-7A7AE9D170FB}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvGraphicFramePr/>
-          </xdr:nvGraphicFramePr>
-          <xdr:xfrm>
-            <a:off x="0" y="0"/>
-            <a:ext cx="0" cy="0"/>
-          </xdr:xfrm>
-          <a:graphic>
-            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
-              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-            </a:graphicData>
-          </a:graphic>
-        </xdr:graphicFrame>
-      </mc:Choice>
-      <mc:Fallback>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="0" name=""/>
-            <xdr:cNvSpPr>
-              <a:spLocks noTextEdit="1"/>
-            </xdr:cNvSpPr>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="3856383" y="917713"/>
-              <a:ext cx="4572000" cy="2743200"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:solidFill>
-              <a:prstClr val="white"/>
-            </a:solidFill>
-            <a:ln w="1">
-              <a:solidFill>
-                <a:prstClr val="green"/>
-              </a:solidFill>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:r>
-                <a:rPr lang="ru-RU" sz="1100"/>
-                <a:t>Эта диаграмма недоступна в вашей версии Excel.
-Изменение этой фигуры или сохранение книги в другом формате приведет к остаточному повреждению диаграммы.</a:t>
-              </a:r>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Fallback>
-    </mc:AlternateContent>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Диаграмма 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{54A7CB2E-DEC3-40E9-A33C-D480BAF30CE5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>602973</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>9939</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>298173</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>155713</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Диаграмма 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C2005B2-0410-465C-BEB3-B71AA23B59FB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>6626</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>168965</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>311426</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>129209</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Диаграмма 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C56BABA-BB1E-4052-969B-23D0BD384F7B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1112,10 +3859,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O23"/>
+  <dimension ref="A1:O37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+    <sheetView tabSelected="1" topLeftCell="H22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="Y37" sqref="Y37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1515,6 +4262,16 @@
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
       <c r="J13" s="1"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="M13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="N13" s="2" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
@@ -1542,6 +4299,18 @@
         <v>16</v>
       </c>
       <c r="J14" s="1"/>
+      <c r="K14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
@@ -1569,6 +4338,18 @@
         <v>0</v>
       </c>
       <c r="J15" s="1"/>
+      <c r="K15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L15">
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="E16" s="1" t="s">
@@ -1585,8 +4366,20 @@
         <v>0</v>
       </c>
       <c r="J16" s="1"/>
+      <c r="K16" t="s">
+        <v>10</v>
+      </c>
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
     </row>
-    <row r="17" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="5:14" x14ac:dyDescent="0.3">
       <c r="E17" t="s">
         <v>10</v>
       </c>
@@ -1602,7 +4395,7 @@
       </c>
       <c r="J17" s="1"/>
     </row>
-    <row r="18" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="5:14" x14ac:dyDescent="0.3">
       <c r="E18" s="1" t="s">
         <v>8</v>
       </c>
@@ -1619,8 +4412,17 @@
         <f>H18</f>
         <v>0.16</v>
       </c>
+      <c r="L18" t="s">
+        <v>13</v>
+      </c>
+      <c r="M18" t="s">
+        <v>17</v>
+      </c>
+      <c r="N18" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="19" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="5:14" x14ac:dyDescent="0.3">
       <c r="E19" s="1" t="s">
         <v>9</v>
       </c>
@@ -1635,8 +4437,20 @@
         <f t="shared" ref="I19:I20" si="1">H19</f>
         <v>0.01</v>
       </c>
+      <c r="K19" t="s">
+        <v>8</v>
+      </c>
+      <c r="L19">
+        <v>0</v>
+      </c>
+      <c r="M19">
+        <v>0.16</v>
+      </c>
+      <c r="N19">
+        <v>0.09</v>
+      </c>
     </row>
-    <row r="20" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="5:14" x14ac:dyDescent="0.3">
       <c r="E20" t="s">
         <v>10</v>
       </c>
@@ -1651,8 +4465,20 @@
         <f t="shared" si="1"/>
         <v>0.01</v>
       </c>
+      <c r="K20" t="s">
+        <v>9</v>
+      </c>
+      <c r="L20">
+        <v>0</v>
+      </c>
+      <c r="M20">
+        <v>0.01</v>
+      </c>
+      <c r="N20">
+        <v>0</v>
+      </c>
     </row>
-    <row r="21" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="5:14" x14ac:dyDescent="0.3">
       <c r="E21" s="1" t="s">
         <v>8</v>
       </c>
@@ -1669,8 +4495,20 @@
         <f>H21</f>
         <v>108.56</v>
       </c>
+      <c r="K21" t="s">
+        <v>10</v>
+      </c>
+      <c r="L21">
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <v>0.01</v>
+      </c>
+      <c r="N21">
+        <v>0</v>
+      </c>
     </row>
-    <row r="22" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="5:14" x14ac:dyDescent="0.3">
       <c r="E22" s="1" t="s">
         <v>9</v>
       </c>
@@ -1686,7 +4524,7 @@
         <v>4.66</v>
       </c>
     </row>
-    <row r="23" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="5:14" x14ac:dyDescent="0.3">
       <c r="E23" t="s">
         <v>10</v>
       </c>
@@ -1700,6 +4538,59 @@
       <c r="I23">
         <f t="shared" si="2"/>
         <v>5.14</v>
+      </c>
+    </row>
+    <row r="34" spans="11:14" x14ac:dyDescent="0.3">
+      <c r="L34" t="s">
+        <v>13</v>
+      </c>
+      <c r="M34" t="s">
+        <v>17</v>
+      </c>
+      <c r="N34" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="35" spans="11:14" x14ac:dyDescent="0.3">
+      <c r="K35" t="s">
+        <v>8</v>
+      </c>
+      <c r="L35">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="M35">
+        <v>108.56</v>
+      </c>
+      <c r="N35">
+        <v>97.22</v>
+      </c>
+    </row>
+    <row r="36" spans="11:14" x14ac:dyDescent="0.3">
+      <c r="K36" t="s">
+        <v>9</v>
+      </c>
+      <c r="L36">
+        <v>2.0299999999999998</v>
+      </c>
+      <c r="M36">
+        <v>4.66</v>
+      </c>
+      <c r="N36">
+        <v>2.4900000000000002</v>
+      </c>
+    </row>
+    <row r="37" spans="11:14" x14ac:dyDescent="0.3">
+      <c r="K37" t="s">
+        <v>10</v>
+      </c>
+      <c r="L37">
+        <v>2.65</v>
+      </c>
+      <c r="M37">
+        <v>5.14</v>
+      </c>
+      <c r="N37">
+        <v>1.86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>